<commit_message>
UPDATE correções e ADD seção Avanço por Roda
</commit_message>
<xml_diff>
--- a/monografia/Assets/analise trator.xlsx
+++ b/monografia/Assets/analise trator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Trator" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="D1_09052015_t7_245" localSheetId="2">'D1'!$A$2:$I$153</definedName>
     <definedName name="D2_09052015_t7_245" localSheetId="3">'D2'!$A$2:$N$38</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -5098,12 +5098,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="69914624"/>
-        <c:axId val="69916544"/>
+        <c:axId val="52477312"/>
+        <c:axId val="52491776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69914624"/>
+        <c:axId val="52477312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5130,12 +5129,12 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69916544"/>
+        <c:crossAx val="52491776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69916544"/>
+        <c:axId val="52491776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2000000000000002"/>
@@ -5164,7 +5163,7 @@
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69914624"/>
+        <c:crossAx val="52477312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5178,7 +5177,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6144,12 +6143,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="95979776"/>
-        <c:axId val="95994240"/>
+        <c:axId val="58300288"/>
+        <c:axId val="58306560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95979776"/>
+        <c:axId val="58300288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6175,12 +6173,12 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95994240"/>
+        <c:crossAx val="58306560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95994240"/>
+        <c:axId val="58306560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6208,7 +6206,7 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95979776"/>
+        <c:crossAx val="58300288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6222,7 +6220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8140,12 +8138,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="96413568"/>
-        <c:axId val="96436224"/>
+        <c:axId val="93603328"/>
+        <c:axId val="93605248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96413568"/>
+        <c:axId val="93603328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8171,12 +8168,12 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96436224"/>
+        <c:crossAx val="93605248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96436224"/>
+        <c:axId val="93605248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8212,7 +8209,7 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96413568"/>
+        <c:crossAx val="93603328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8226,7 +8223,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11087,12 +11084,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="97790592"/>
-        <c:axId val="97800960"/>
+        <c:axId val="93919488"/>
+        <c:axId val="93925760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97790592"/>
+        <c:axId val="93919488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11118,12 +11114,12 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97800960"/>
+        <c:crossAx val="93925760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97800960"/>
+        <c:axId val="93925760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -11159,7 +11155,7 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97790592"/>
+        <c:crossAx val="93919488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11173,7 +11169,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -15944,12 +15940,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="99510144"/>
-        <c:axId val="99528704"/>
+        <c:axId val="95385088"/>
+        <c:axId val="95387008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99510144"/>
+        <c:axId val="95385088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15975,12 +15970,12 @@
         <c:numFmt formatCode="Geral" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99528704"/>
+        <c:crossAx val="95387008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99528704"/>
+        <c:axId val="95387008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -16008,7 +16003,7 @@
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99510144"/>
+        <c:crossAx val="95385088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16022,7 +16017,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -16486,7 +16481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
@@ -16721,8 +16716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y528"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>